<commit_message>
Updated 2020-03-31 with data from 2020-03-30
</commit_message>
<xml_diff>
--- a/country-continent.xlsx
+++ b/country-continent.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lasse\Google Drive\ITU\DATAVISUALISATION\Lecture 9 - data journalism\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2FFA0F8C-BEC1-42B3-9D35-2512F00E1B32}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B5ED7478-350C-431A-8999-4A10901EA4E1}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1290" yWindow="1365" windowWidth="27390" windowHeight="12930" xr2:uid="{C6ACBE00-5C57-42A0-8DE6-97A73C2380C9}"/>
+    <workbookView xWindow="390" yWindow="390" windowWidth="25770" windowHeight="13080" xr2:uid="{C6ACBE00-5C57-42A0-8DE6-97A73C2380C9}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="356" uniqueCount="186">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="358" uniqueCount="187">
   <si>
     <t>Togo</t>
   </si>
@@ -589,6 +589,9 @@
   </si>
   <si>
     <t>Timor-Leste</t>
+  </si>
+  <si>
+    <t>Botswana</t>
   </si>
 </sst>
 </file>
@@ -940,10 +943,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{28DEAFAE-CA04-4A91-A7D0-E8A41B987F5B}">
-  <dimension ref="A1:B178"/>
+  <dimension ref="A1:B179"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A163" workbookViewId="0">
-      <selection activeCell="B178" sqref="B178"/>
+      <selection activeCell="B179" sqref="B179"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2376,6 +2379,14 @@
         <v>6</v>
       </c>
     </row>
+    <row r="179" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A179" t="s">
+        <v>186</v>
+      </c>
+      <c r="B179" t="s">
+        <v>1</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>